<commit_message>
list 최종, description 수정
</commit_message>
<xml_diff>
--- a/Requirement List/requriementList(+description)_ByunBogyeong.xlsx
+++ b/Requirement List/requriementList(+description)_ByunBogyeong.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\소공\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SW_engineering_13_group\Requirement List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2472EBDA-9834-4FB7-B8A9-035FE121052E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00BEEE-E200-4542-B259-B731547987DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15D10122-E891-4960-AD69-6842C183E103}"/>
   </bookViews>
@@ -418,18 +418,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2. 관리자 및 회원 로그인, 회원 가입 메뉴를 띄운다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. 관리자 로그인 메뉴를 누른다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. 관리자 로그인 화면을 띄운다.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>6. 관리자용 메뉴를 띄운다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -533,6 +521,18 @@
   </si>
   <si>
     <t>자전거 상세 정보 조회</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 로그인, 회원 가입 메뉴를 띄운다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 로그인 메뉴를 누른다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 로그인 화면을 띄운다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -650,7 +650,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -663,7 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -675,23 +675,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1027,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B74E6A7-CA28-464D-AAD9-9607B7B145D5}">
-  <dimension ref="A2:H49"/>
+  <dimension ref="C2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1148,69 +1142,69 @@
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.4">
       <c r="D14" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.4">
       <c r="D15" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.4">
       <c r="D16" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="28.8" x14ac:dyDescent="0.4">
       <c r="D17" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.4">
@@ -1248,78 +1242,78 @@
         <v>22</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D22" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D23" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D24" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="4:8" ht="28.8" x14ac:dyDescent="0.4">
       <c r="D25" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="4:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D26" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E26" s="11"/>
       <c r="G26" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H26" s="11"/>
     </row>
@@ -1335,7 +1329,7 @@
       </c>
       <c r="E28" s="6"/>
       <c r="G28" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H28" s="6"/>
     </row>
@@ -1358,136 +1352,126 @@
         <v>22</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D31" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D32" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" ht="43.2" x14ac:dyDescent="0.4">
+      <c r="D34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.4">
-      <c r="D34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G34" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D40" s="4"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.4">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.4">
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D45" s="4"/>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="4:8" x14ac:dyDescent="0.4">
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.4">
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>